<commit_message>
subiendo archivos semana 3
</commit_message>
<xml_diff>
--- a/road_map_grupo_1_s3.xlsx
+++ b/road_map_grupo_1_s3.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EEBEDC-E35A-4280-91A1-01A2E4BA1F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9378D734-5AEE-4F56-9CE8-3F8B95544B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1845" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RoadMap FINAL" sheetId="11" r:id="rId1"/>
@@ -1000,7 +1000,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -1071,119 +1071,113 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="22" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="25" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="20" fillId="25" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="25" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="25" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="22" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="22" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="25" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="24" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="24" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="22" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="25" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="25" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="25" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="25" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="25" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="22" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="22" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1230,77 +1224,7 @@
     <cellStyle name="Título 3" xfId="32" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -3585,8 +3509,8 @@
   </sheetPr>
   <dimension ref="B1:X33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Y20" sqref="Y20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -3672,9 +3596,9 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
@@ -3692,103 +3616,103 @@
     <row r="5" spans="2:24" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="61" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="21"/>
-      <c r="F5" s="59" t="s">
+      <c r="F5" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="60"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="43" t="s">
+      <c r="G5" s="49"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43" t="s">
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43" t="s">
+      <c r="M5" s="53"/>
+      <c r="N5" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="43"/>
-      <c r="P5" s="58" t="s">
+      <c r="O5" s="53"/>
+      <c r="P5" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="Q5" s="43" t="s">
+      <c r="Q5" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="R5" s="43"/>
-      <c r="S5" s="58" t="s">
+      <c r="R5" s="53"/>
+      <c r="S5" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="T5" s="43" t="s">
+      <c r="T5" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="U5" s="43"/>
-      <c r="V5" s="43" t="s">
+      <c r="U5" s="53"/>
+      <c r="V5" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="W5" s="43"/>
+      <c r="W5" s="53"/>
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="2:24" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="28"/>
+      <c r="D6" s="61"/>
       <c r="E6" s="21"/>
-      <c r="F6" s="42" t="s">
+      <c r="F6" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="42" t="s">
+      <c r="G6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="42" t="s">
+      <c r="H6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="42" t="s">
+      <c r="I6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="42" t="s">
+      <c r="J6" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="42" t="s">
+      <c r="K6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="42" t="s">
+      <c r="L6" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="42" t="s">
+      <c r="M6" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="42" t="s">
+      <c r="N6" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="62" t="s">
+      <c r="O6" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="42" t="s">
+      <c r="P6" s="52"/>
+      <c r="Q6" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="R6" s="42" t="s">
+      <c r="R6" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="S6" s="42" t="s">
+      <c r="S6" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="T6" s="42" t="s">
+      <c r="T6" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="U6" s="42" t="s">
+      <c r="U6" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="V6" s="42" t="s">
+      <c r="V6" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="W6" s="42" t="s">
+      <c r="W6" s="28" t="s">
         <v>30</v>
       </c>
       <c r="X6" s="1"/>
@@ -3815,13 +3739,13 @@
       <c r="T7" s="9"/>
       <c r="U7" s="17"/>
       <c r="V7" s="9"/>
-      <c r="W7" s="39"/>
+      <c r="W7" s="19"/>
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="2:24" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="54" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="20"/>
@@ -3830,7 +3754,7 @@
       <c r="H8" s="23"/>
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
-      <c r="K8" s="44"/>
+      <c r="K8" s="30"/>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
       <c r="N8" s="18"/>
@@ -3842,20 +3766,20 @@
       <c r="T8" s="18"/>
       <c r="U8" s="18"/>
       <c r="V8" s="13"/>
-      <c r="W8" s="44"/>
+      <c r="W8" s="30"/>
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="2:24" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="30"/>
+      <c r="D9" s="55"/>
       <c r="E9" s="20"/>
       <c r="F9" s="23"/>
       <c r="G9" s="13"/>
       <c r="H9" s="23"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
-      <c r="K9" s="38"/>
+      <c r="K9" s="27"/>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
       <c r="N9" s="14"/>
@@ -3867,7 +3791,7 @@
       <c r="T9" s="14"/>
       <c r="U9" s="14"/>
       <c r="V9" s="13"/>
-      <c r="W9" s="38"/>
+      <c r="W9" s="27"/>
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="2:24" ht="18" x14ac:dyDescent="0.3">
@@ -3898,7 +3822,7 @@
     <row r="11" spans="2:24" ht="18" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="56" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="22"/>
@@ -3907,7 +3831,7 @@
       <c r="H11" s="23"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
-      <c r="K11" s="38"/>
+      <c r="K11" s="27"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
       <c r="N11" s="18"/>
@@ -3919,20 +3843,20 @@
       <c r="T11" s="18"/>
       <c r="U11" s="18"/>
       <c r="V11" s="13"/>
-      <c r="W11" s="44"/>
+      <c r="W11" s="30"/>
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="2:24" ht="18" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="32"/>
+      <c r="D12" s="57"/>
       <c r="E12" s="20"/>
       <c r="F12" s="23"/>
       <c r="G12" s="13"/>
       <c r="H12" s="23"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
-      <c r="K12" s="38"/>
+      <c r="K12" s="27"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
       <c r="N12" s="14"/>
@@ -3944,20 +3868,20 @@
       <c r="T12" s="14"/>
       <c r="U12" s="14"/>
       <c r="V12" s="13"/>
-      <c r="W12" s="48"/>
+      <c r="W12" s="34"/>
       <c r="X12" s="1"/>
     </row>
     <row r="13" spans="2:24" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="33"/>
+      <c r="D13" s="58"/>
       <c r="E13" s="20"/>
       <c r="F13" s="23"/>
       <c r="G13" s="13"/>
       <c r="H13" s="23"/>
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
-      <c r="K13" s="38"/>
+      <c r="K13" s="27"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
       <c r="N13" s="16"/>
@@ -3969,7 +3893,7 @@
       <c r="T13" s="16"/>
       <c r="U13" s="16"/>
       <c r="V13" s="13"/>
-      <c r="W13" s="38"/>
+      <c r="W13" s="27"/>
       <c r="X13" s="1"/>
     </row>
     <row r="14" spans="2:24" ht="18" x14ac:dyDescent="0.3">
@@ -4000,7 +3924,7 @@
     <row r="15" spans="2:24" ht="18" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="44" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="22"/>
@@ -4021,13 +3945,13 @@
       <c r="T15" s="18"/>
       <c r="U15" s="18"/>
       <c r="V15" s="13"/>
-      <c r="W15" s="44"/>
+      <c r="W15" s="30"/>
       <c r="X15" s="1"/>
     </row>
     <row r="16" spans="2:24" ht="18" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="35"/>
+      <c r="D16" s="59"/>
       <c r="E16" s="20"/>
       <c r="F16" s="23"/>
       <c r="G16" s="13"/>
@@ -4046,13 +3970,13 @@
       <c r="T16" s="14"/>
       <c r="U16" s="14"/>
       <c r="V16" s="13"/>
-      <c r="W16" s="48"/>
+      <c r="W16" s="34"/>
       <c r="X16" s="1"/>
     </row>
     <row r="17" spans="2:24" ht="136.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="36"/>
+      <c r="D17" s="60"/>
       <c r="E17" s="20"/>
       <c r="F17" s="23"/>
       <c r="G17" s="13"/>
@@ -4071,7 +3995,7 @@
       <c r="T17" s="16"/>
       <c r="U17" s="16"/>
       <c r="V17" s="13"/>
-      <c r="W17" s="38"/>
+      <c r="W17" s="27"/>
       <c r="X17" s="1"/>
     </row>
     <row r="18" spans="2:24" ht="18" x14ac:dyDescent="0.3">
@@ -4102,7 +4026,7 @@
     <row r="19" spans="2:24" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="56" t="s">
         <v>31</v>
       </c>
       <c r="E19" s="22"/>
@@ -4123,13 +4047,13 @@
       <c r="T19" s="18"/>
       <c r="U19" s="18"/>
       <c r="V19" s="13"/>
-      <c r="W19" s="44"/>
+      <c r="W19" s="30"/>
       <c r="X19" s="1"/>
     </row>
     <row r="20" spans="2:24" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="27"/>
+      <c r="D20" s="47"/>
       <c r="E20" s="20"/>
       <c r="F20" s="23"/>
       <c r="G20" s="13"/>
@@ -4148,7 +4072,7 @@
       <c r="T20" s="16"/>
       <c r="U20" s="16"/>
       <c r="V20" s="13"/>
-      <c r="W20" s="38"/>
+      <c r="W20" s="27"/>
       <c r="X20" s="1"/>
     </row>
     <row r="21" spans="2:24" ht="18" x14ac:dyDescent="0.3">
@@ -4179,7 +4103,7 @@
     <row r="22" spans="2:24" ht="18" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="44" t="s">
         <v>32</v>
       </c>
       <c r="E22" s="20"/>
@@ -4191,66 +4115,66 @@
       <c r="K22" s="18"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
-      <c r="N22" s="47"/>
-      <c r="O22" s="47"/>
+      <c r="N22" s="33"/>
+      <c r="O22" s="33"/>
       <c r="P22" s="13"/>
-      <c r="Q22" s="47"/>
-      <c r="R22" s="47"/>
+      <c r="Q22" s="33"/>
+      <c r="R22" s="33"/>
       <c r="S22" s="13"/>
-      <c r="T22" s="47"/>
-      <c r="U22" s="47"/>
+      <c r="T22" s="33"/>
+      <c r="U22" s="33"/>
       <c r="V22" s="13"/>
-      <c r="W22" s="44"/>
+      <c r="W22" s="30"/>
       <c r="X22" s="1"/>
     </row>
     <row r="23" spans="2:24" ht="18" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="41"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="20"/>
       <c r="F23" s="23"/>
       <c r="G23" s="13"/>
       <c r="H23" s="23"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="46"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
-      <c r="N23" s="48"/>
-      <c r="O23" s="48"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
       <c r="P23" s="13"/>
-      <c r="Q23" s="48"/>
-      <c r="R23" s="48"/>
+      <c r="Q23" s="34"/>
+      <c r="R23" s="34"/>
       <c r="S23" s="13"/>
-      <c r="T23" s="48"/>
-      <c r="U23" s="48"/>
+      <c r="T23" s="34"/>
+      <c r="U23" s="34"/>
       <c r="V23" s="13"/>
-      <c r="W23" s="48"/>
+      <c r="W23" s="34"/>
       <c r="X23" s="1"/>
     </row>
     <row r="24" spans="2:24" ht="18" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="41"/>
+      <c r="D24" s="45"/>
       <c r="E24" s="20"/>
       <c r="F24" s="23"/>
       <c r="G24" s="13"/>
       <c r="H24" s="23"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="38"/>
-      <c r="P24" s="37"/>
-      <c r="Q24" s="38"/>
-      <c r="R24" s="38"/>
-      <c r="S24" s="37"/>
-      <c r="T24" s="38"/>
-      <c r="U24" s="38"/>
-      <c r="V24" s="37"/>
-      <c r="W24" s="38"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="27"/>
+      <c r="R24" s="27"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="27"/>
+      <c r="V24" s="26"/>
+      <c r="W24" s="27"/>
       <c r="X24" s="1"/>
     </row>
     <row r="25" spans="2:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4281,7 +4205,7 @@
     <row r="26" spans="2:24" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="46" t="s">
         <v>33</v>
       </c>
       <c r="E26" s="22"/>
@@ -4302,13 +4226,13 @@
       <c r="T26" s="18"/>
       <c r="U26" s="18"/>
       <c r="V26" s="13"/>
-      <c r="W26" s="44"/>
+      <c r="W26" s="30"/>
       <c r="X26" s="1"/>
     </row>
     <row r="27" spans="2:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="27"/>
+      <c r="D27" s="47"/>
       <c r="E27" s="20"/>
       <c r="F27" s="23"/>
       <c r="G27" s="13"/>
@@ -4327,7 +4251,7 @@
       <c r="T27" s="16"/>
       <c r="U27" s="16"/>
       <c r="V27" s="13"/>
-      <c r="W27" s="38"/>
+      <c r="W27" s="27"/>
       <c r="X27" s="1"/>
     </row>
     <row r="28" spans="2:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4358,78 +4282,78 @@
     <row r="29" spans="2:24" ht="93" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="34" t="s">
+      <c r="D29" s="44" t="s">
         <v>34</v>
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="23"/>
       <c r="G29" s="13"/>
       <c r="H29" s="23"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="44"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="30"/>
       <c r="L29" s="13"/>
       <c r="M29" s="13"/>
-      <c r="N29" s="47"/>
-      <c r="O29" s="47"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="33"/>
       <c r="P29" s="13"/>
-      <c r="Q29" s="47"/>
-      <c r="R29" s="47"/>
+      <c r="Q29" s="33"/>
+      <c r="R29" s="33"/>
       <c r="S29" s="13"/>
-      <c r="T29" s="47"/>
-      <c r="U29" s="47"/>
+      <c r="T29" s="33"/>
+      <c r="U29" s="33"/>
       <c r="V29" s="13"/>
-      <c r="W29" s="38"/>
+      <c r="W29" s="27"/>
       <c r="X29" s="1"/>
     </row>
     <row r="30" spans="2:24" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="41"/>
+      <c r="D30" s="45"/>
       <c r="E30" s="20"/>
       <c r="F30" s="13"/>
-      <c r="G30" s="56"/>
+      <c r="G30" s="42"/>
       <c r="H30" s="13"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="50"/>
-      <c r="L30" s="55"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="41"/>
       <c r="M30" s="13"/>
-      <c r="N30" s="48"/>
-      <c r="O30" s="48"/>
+      <c r="N30" s="34"/>
+      <c r="O30" s="34"/>
       <c r="P30" s="13"/>
-      <c r="Q30" s="48"/>
-      <c r="R30" s="48"/>
-      <c r="S30" s="53"/>
-      <c r="T30" s="49"/>
-      <c r="U30" s="50"/>
-      <c r="V30" s="37"/>
-      <c r="W30" s="38"/>
+      <c r="Q30" s="34"/>
+      <c r="R30" s="34"/>
+      <c r="S30" s="39"/>
+      <c r="T30" s="35"/>
+      <c r="U30" s="36"/>
+      <c r="V30" s="26"/>
+      <c r="W30" s="27"/>
       <c r="X30" s="1"/>
     </row>
     <row r="31" spans="2:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="41"/>
+      <c r="D31" s="45"/>
       <c r="E31" s="20"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="52"/>
-      <c r="L31" s="37"/>
-      <c r="M31" s="37"/>
-      <c r="N31" s="38"/>
-      <c r="O31" s="38"/>
-      <c r="P31" s="37"/>
-      <c r="Q31" s="38"/>
-      <c r="R31" s="38"/>
-      <c r="S31" s="37"/>
-      <c r="T31" s="38"/>
-      <c r="U31" s="38"/>
-      <c r="V31" s="54"/>
-      <c r="W31" s="38"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="27"/>
+      <c r="O31" s="27"/>
+      <c r="P31" s="26"/>
+      <c r="Q31" s="27"/>
+      <c r="R31" s="27"/>
+      <c r="S31" s="26"/>
+      <c r="T31" s="27"/>
+      <c r="U31" s="27"/>
+      <c r="V31" s="40"/>
+      <c r="W31" s="27"/>
       <c r="X31" s="1"/>
     </row>
     <row r="32" spans="2:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4485,100 +4409,60 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="16">
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="Q5:R5"/>
     <mergeCell ref="D22:D24"/>
     <mergeCell ref="D26:D27"/>
     <mergeCell ref="D29:D31"/>
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="O6:P6"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="D15:D17"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="Q5:R5"/>
   </mergeCells>
-  <conditionalFormatting sqref="Q8:S24 T8:U31 W8:W31 V8:V24 F9:K19 F25:S25 F8:O8 F28:S28 F32:W33 F29:R31 F20:O21 F27:O27 F24:K24 F26:K26">
-    <cfRule type="expression" dxfId="19" priority="21">
+  <conditionalFormatting sqref="F8:O8 Q8:S24 F9:K19 F32:W33">
+    <cfRule type="expression" dxfId="9" priority="21">
       <formula>AND(#REF!&gt;5%, #REF!&lt;=#REF!,ROUNDDOWN(NETWORKDAYS(#REF!,#REF!)*#REF!,0)+#REF!+1&gt;=#REF!)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="22">
+    <cfRule type="expression" dxfId="8" priority="22">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=#REF!,#REF!&gt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L9:O9 L10 P8:P9 N10:P10 P11:P24 L26:O26 P26:R27 V25 V28 L11:O19 L22:O24">
-    <cfRule type="expression" dxfId="17" priority="19">
+  <conditionalFormatting sqref="F20:O24">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>AND(#REF!&gt;5%, #REF!&lt;=#REF!,ROUNDDOWN(NETWORKDAYS(#REF!,#REF!)*#REF!,0)+#REF!+1&gt;=#REF!)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="20">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=#REF!,#REF!&gt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S26:S27">
-    <cfRule type="expression" dxfId="15" priority="15">
+  <conditionalFormatting sqref="F25:S31">
+    <cfRule type="expression" dxfId="5" priority="13">
       <formula>AND(#REF!&gt;5%, #REF!&lt;=#REF!,ROUNDDOWN(NETWORKDAYS(#REF!,#REF!)*#REF!,0)+#REF!+1&gt;=#REF!)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="16">
+    <cfRule type="expression" dxfId="4" priority="14">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=#REF!,#REF!&gt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S29:S31">
-    <cfRule type="expression" dxfId="13" priority="13">
+  <conditionalFormatting sqref="P8:P9 L9:O9 L10 N10:P10 L11:O19 P11:P24">
+    <cfRule type="expression" dxfId="3" priority="19">
       <formula>AND(#REF!&gt;5%, #REF!&lt;=#REF!,ROUNDDOWN(NETWORKDAYS(#REF!,#REF!)*#REF!,0)+#REF!+1&gt;=#REF!)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="2" priority="20">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=#REF!,#REF!&gt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V26:V27">
-    <cfRule type="expression" dxfId="11" priority="11">
+  <conditionalFormatting sqref="T8:W31">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>AND(#REF!&gt;5%, #REF!&lt;=#REF!,ROUNDDOWN(NETWORKDAYS(#REF!,#REF!)*#REF!,0)+#REF!+1&gt;=#REF!)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
-      <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=#REF!,#REF!&gt;=#REF!)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V29:V31">
-    <cfRule type="expression" dxfId="9" priority="9">
-      <formula>AND(#REF!&gt;5%, #REF!&lt;=#REF!,ROUNDDOWN(NETWORKDAYS(#REF!,#REF!)*#REF!,0)+#REF!+1&gt;=#REF!)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10">
-      <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=#REF!,#REF!&gt;=#REF!)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F22:H22">
-    <cfRule type="expression" dxfId="7" priority="7">
-      <formula>AND(#REF!&gt;5%, #REF!&lt;=#REF!,ROUNDDOWN(NETWORKDAYS(#REF!,#REF!)*#REF!,0)+#REF!+1&gt;=#REF!)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
-      <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=#REF!,#REF!&gt;=#REF!)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F23:H23">
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>AND(#REF!&gt;5%, #REF!&lt;=#REF!,ROUNDDOWN(NETWORKDAYS(#REF!,#REF!)*#REF!,0)+#REF!+1&gt;=#REF!)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
-      <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=#REF!,#REF!&gt;=#REF!)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I23:K23">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>AND(#REF!&gt;5%, #REF!&lt;=#REF!,ROUNDDOWN(NETWORKDAYS(#REF!,#REF!)*#REF!,0)+#REF!+1&gt;=#REF!)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=#REF!,#REF!&gt;=#REF!)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I22:K22">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>AND(#REF!&gt;5%, #REF!&lt;=#REF!,ROUNDDOWN(NETWORKDAYS(#REF!,#REF!)*#REF!,0)+#REF!+1&gt;=#REF!)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="0" priority="10">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=#REF!,#REF!&gt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>